<commit_message>
upated missing input and testplan
</commit_message>
<xml_diff>
--- a/test-plan.xlsx
+++ b/test-plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCU\SELAB\student-result-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4A6B55-3DE8-4483-8E90-6DCC779B914F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E342832-006A-4B67-B90C-5BFB40DF5646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="102">
   <si>
     <t xml:space="preserve"> Test Plan</t>
   </si>
@@ -102,12 +102,6 @@
     <t>Prompts to skip</t>
   </si>
   <si>
-    <t>User chooses not to skip</t>
-  </si>
-  <si>
-    <t>Invalid record + 'n'</t>
-  </si>
-  <si>
     <t>Program stops</t>
   </si>
   <si>
@@ -271,13 +265,79 @@
   </si>
   <si>
     <t>Displayed Error message</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>terminates</t>
+  </si>
+  <si>
+    <t>wrong input</t>
+  </si>
+  <si>
+    <t>Ask skip: user wrong input</t>
+  </si>
+  <si>
+    <t>Store student details</t>
+  </si>
+  <si>
+    <t>Valid ID and name</t>
+  </si>
+  <si>
+    <t>Data stored correctly</t>
+  </si>
+  <si>
+    <t>Stored correctly</t>
+  </si>
+  <si>
+    <t>Store subject marks</t>
+  </si>
+  <si>
+    <t>5 subjects with marks</t>
+  </si>
+  <si>
+    <t>All subjects stored</t>
+  </si>
+  <si>
+    <t>Stored</t>
+  </si>
+  <si>
+    <t>Update results</t>
+  </si>
+  <si>
+    <t>Data from compute module</t>
+  </si>
+  <si>
+    <t>Total, CGPA updated</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>Use data for output</t>
+  </si>
+  <si>
+    <t>Student record</t>
+  </si>
+  <si>
+    <t>Correct values printed</t>
+  </si>
+  <si>
+    <t>Printed correctly</t>
+  </si>
+  <si>
+    <t>Output file missing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./result input.txt missing.txt </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +368,14 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -327,7 +395,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -419,11 +487,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -523,6 +617,29 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -832,8 +949,8 @@
   </sheetPr>
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1157,16 +1274,16 @@
         <v>46042</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>12</v>
@@ -1502,8 +1619,8 @@
   </sheetPr>
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="A7:G11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1511,7 +1628,7 @@
     <col min="1" max="1" width="14.54296875" style="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.54296875" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.54296875" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7265625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.453125" style="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.1796875" style="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.81640625" style="23" bestFit="1" customWidth="1"/>
@@ -1647,19 +1764,19 @@
       <c r="B6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="27" t="s">
         <v>7</v>
       </c>
       <c r="H6" s="3"/>
@@ -1682,25 +1799,25 @@
       <c r="A7" s="13">
         <v>1</v>
       </c>
-      <c r="B7" s="14">
-        <v>46042</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="15" t="s">
+      <c r="B7" s="45">
+        <v>46044</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="H7" s="24"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1720,25 +1837,25 @@
       <c r="A8" s="13">
         <v>2</v>
       </c>
-      <c r="B8" s="14">
-        <v>46042</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="15" t="s">
+      <c r="B8" s="45">
+        <v>46044</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="3"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1758,25 +1875,25 @@
       <c r="A9" s="13">
         <v>3</v>
       </c>
-      <c r="B9" s="14">
-        <v>46042</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="15" t="s">
+      <c r="B9" s="45">
+        <v>46044</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="3"/>
+      <c r="H9" s="24"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1796,25 +1913,25 @@
       <c r="A10" s="13">
         <v>4</v>
       </c>
-      <c r="B10" s="14">
-        <v>46042</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="15" t="s">
+      <c r="B10" s="45">
+        <v>46044</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="3"/>
+      <c r="H10" s="24"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -1831,27 +1948,13 @@
       <c r="V10" s="3"/>
     </row>
     <row r="11" spans="1:22" ht="18.75" customHeight="1">
-      <c r="A11" s="13">
-        <v>5</v>
-      </c>
-      <c r="B11" s="14">
-        <v>46042</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>12</v>
-      </c>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -1869,12 +1972,12 @@
       <c r="V11" s="3"/>
     </row>
     <row r="12" spans="1:22" ht="18.75" customHeight="1">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
       <c r="G12" s="15"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -1893,25 +1996,13 @@
       <c r="V12" s="3"/>
     </row>
     <row r="13" spans="1:22" ht="18.75" customHeight="1">
-      <c r="A13" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="20" t="s">
+      <c r="A13" s="42"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="37" t="s">
         <v>8</v>
       </c>
       <c r="H13" s="3"/>
@@ -1931,19 +2022,13 @@
       <c r="V13" s="3"/>
     </row>
     <row r="14" spans="1:22" ht="22" customHeight="1">
-      <c r="A14" s="16"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="15"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="38"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -1961,19 +2046,13 @@
       <c r="V14" s="3"/>
     </row>
     <row r="15" spans="1:22" ht="22" customHeight="1">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="15"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="38"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -1991,19 +2070,13 @@
       <c r="V15" s="3"/>
     </row>
     <row r="16" spans="1:22" ht="22" customHeight="1">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="15"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="38"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -2021,19 +2094,13 @@
       <c r="V16" s="3"/>
     </row>
     <row r="17" spans="1:22" ht="22" customHeight="1">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="15"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="38"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -2051,12 +2118,12 @@
       <c r="V17" s="3"/>
     </row>
     <row r="18" spans="1:22" ht="22" customHeight="1">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
       <c r="G18" s="15"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -2356,16 +2423,16 @@
         <v>46042</v>
       </c>
       <c r="C7" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="F7" s="31" t="s">
         <v>29</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>31</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>12</v>
@@ -2394,16 +2461,16 @@
         <v>46042</v>
       </c>
       <c r="C8" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>34</v>
-      </c>
       <c r="F8" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>12</v>
@@ -2432,16 +2499,16 @@
         <v>46042</v>
       </c>
       <c r="C9" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="F9" s="31" t="s">
         <v>36</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>38</v>
       </c>
       <c r="G9" s="31" t="s">
         <v>12</v>
@@ -2470,16 +2537,16 @@
         <v>46042</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="31" t="s">
         <v>39</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>41</v>
       </c>
       <c r="G10" s="31" t="s">
         <v>12</v>
@@ -2988,16 +3055,16 @@
         <v>46042</v>
       </c>
       <c r="C7" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>44</v>
-      </c>
       <c r="F7" s="31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>12</v>
@@ -3026,16 +3093,16 @@
         <v>46042</v>
       </c>
       <c r="C8" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>47</v>
-      </c>
       <c r="F8" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>12</v>
@@ -3064,16 +3131,16 @@
         <v>46042</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G9" s="31" t="s">
         <v>12</v>
@@ -3102,16 +3169,16 @@
         <v>46042</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" s="31" t="s">
         <v>12</v>
@@ -3140,16 +3207,16 @@
         <v>46042</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G11" s="31" t="s">
         <v>12</v>
@@ -3178,16 +3245,16 @@
         <v>46042</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F12" s="31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G12" s="31" t="s">
         <v>12</v>
@@ -3216,16 +3283,16 @@
         <v>46042</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G13" s="31" t="s">
         <v>12</v>
@@ -3470,7 +3537,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3642,16 +3709,16 @@
         <v>46042</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F7" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>12</v>
@@ -3680,16 +3747,16 @@
         <v>46042</v>
       </c>
       <c r="C8" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>62</v>
-      </c>
       <c r="F8" s="31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>12</v>
@@ -3718,16 +3785,16 @@
         <v>46042</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G9" s="31" t="s">
         <v>12</v>
@@ -3749,13 +3816,27 @@
       <c r="V9" s="3"/>
     </row>
     <row r="10" spans="1:22" ht="18.75" customHeight="1">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="A10" s="31">
+        <v>4</v>
+      </c>
+      <c r="B10" s="32">
+        <v>46043</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>80</v>
+      </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -4112,7 +4193,7 @@
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4284,16 +4365,16 @@
         <v>46042</v>
       </c>
       <c r="C7" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="31" t="s">
         <v>64</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>66</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>12</v>
@@ -4322,16 +4403,16 @@
         <v>46042</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>12</v>
@@ -4360,16 +4441,16 @@
         <v>46042</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="31" t="s">
-        <v>70</v>
-      </c>
       <c r="F9" s="31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G9" s="31" t="s">
         <v>12</v>
@@ -4398,16 +4479,16 @@
         <v>46042</v>
       </c>
       <c r="C10" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="31" t="s">
         <v>71</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>73</v>
       </c>
       <c r="G10" s="31" t="s">
         <v>12</v>

</xml_diff>